<commit_message>
BOM and CPL: removed Switches
Not cost effective

Signed-off-by: Dylan Turner <dylantdmt@gmail.com>
</commit_message>
<xml_diff>
--- a/pcb/parts/FightKey-CPL.xlsx
+++ b/pcb/parts/FightKey-CPL.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="95">
   <si>
     <t xml:space="preserve">Designator</t>
   </si>
@@ -37,33 +37,18 @@
     <t xml:space="preserve">Rot</t>
   </si>
   <si>
-    <t xml:space="preserve">AK_BTN1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">183.515mm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">114.3mm</t>
+    <t xml:space="preserve">C1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">127.6096mm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">64.1604mm</t>
   </si>
   <si>
     <t xml:space="preserve">top</t>
   </si>
   <si>
-    <t xml:space="preserve">AP_BTN1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">75.565mm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">C1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">127.6096mm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">64.1604mm</t>
-  </si>
-  <si>
     <t xml:space="preserve">C2</t>
   </si>
   <si>
@@ -199,63 +184,6 @@
     <t xml:space="preserve">63.91mm</t>
   </si>
   <si>
-    <t xml:space="preserve">DOWN_BTN1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">79.727511mm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">98.425mm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HK_BTN1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">161.925mm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">105.41mm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HP_BTN1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">66.675mm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LEFT_BTN1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">61.030023mm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">87.63mm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LK_BTN1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">118.11mm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">123.19mm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LP_BTN1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">84.455mm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MK_BTN1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">139.7mm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MP_BTN1</t>
-  </si>
-  <si>
     <t xml:space="preserve">R1</t>
   </si>
   <si>
@@ -337,27 +265,6 @@
     <t xml:space="preserve">67.945mm</t>
   </si>
   <si>
-    <t xml:space="preserve">RIGHT_BTN1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">109.22mm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SELECT_BTN1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">71.755mm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">58.42mm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">START_BTN1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">94.615mm</t>
-  </si>
-  <si>
     <t xml:space="preserve">SW_BOOT1</t>
   </si>
   <si>
@@ -380,12 +287,6 @@
   </si>
   <si>
     <t xml:space="preserve">108.047631mm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UP_BTN1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">90.522511mm</t>
   </si>
   <si>
     <t xml:space="preserve">USB1</t>
@@ -504,7 +405,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -521,11 +422,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -549,7 +454,7 @@
   <dimension ref="A1:E48"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+      <selection pane="topLeft" activeCell="F34" activeCellId="0" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -593,7 +498,7 @@
         <v>8</v>
       </c>
       <c r="E2" s="3" t="n">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -601,10 +506,10 @@
         <v>9</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>8</v>
@@ -615,30 +520,30 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="C4" s="3" t="s">
+        <v>14</v>
+      </c>
       <c r="D4" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="3" t="n">
-        <v>180</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>16</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>17</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>8</v>
@@ -649,121 +554,121 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>19</v>
       </c>
+      <c r="C6" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="D6" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E6" s="3" t="n">
-        <v>0</v>
+        <v>270</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>22</v>
       </c>
+      <c r="C7" s="3" t="s">
+        <v>23</v>
+      </c>
       <c r="D7" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E7" s="3" t="n">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E8" s="3" t="n">
-        <v>270</v>
+        <v>180</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E9" s="3" t="n">
-        <v>180</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E10" s="3" t="n">
-        <v>180</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E11" s="3" t="n">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E12" s="3" t="n">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -791,24 +696,24 @@
         <v>42</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E14" s="3" t="n">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>43</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>45</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>8</v>
@@ -831,7 +736,7 @@
         <v>8</v>
       </c>
       <c r="E16" s="3" t="n">
-        <v>90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -839,16 +744,16 @@
         <v>49</v>
       </c>
       <c r="B17" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>48</v>
-      </c>
       <c r="D17" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E17" s="3" t="n">
-        <v>90</v>
+        <v>180</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -865,7 +770,7 @@
         <v>8</v>
       </c>
       <c r="E18" s="3" t="n">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -873,33 +778,33 @@
         <v>54</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E19" s="3" t="n">
-        <v>180</v>
+        <v>270</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>58</v>
-      </c>
       <c r="D20" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E20" s="3" t="n">
-        <v>90</v>
+        <v>270</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -916,7 +821,7 @@
         <v>8</v>
       </c>
       <c r="E21" s="3" t="n">
-        <v>330</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -933,7 +838,7 @@
         <v>8</v>
       </c>
       <c r="E22" s="3" t="n">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -941,16 +846,16 @@
         <v>65</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>66</v>
+        <v>40</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E23" s="3" t="n">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -967,7 +872,7 @@
         <v>8</v>
       </c>
       <c r="E24" s="3" t="n">
-        <v>330</v>
+        <v>270</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -984,7 +889,7 @@
         <v>8</v>
       </c>
       <c r="E25" s="3" t="n">
-        <v>0</v>
+        <v>270</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -992,10 +897,10 @@
         <v>73</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>8</v>
@@ -1006,98 +911,98 @@
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>64</v>
+        <v>78</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E27" s="3" t="n">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E28" s="3" t="n">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="3" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E29" s="3" t="n">
-        <v>270</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E30" s="3" t="n">
-        <v>270</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="3" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>84</v>
+        <v>37</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="D31" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E31" s="3" t="n">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="3" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>8</v>
@@ -1108,265 +1013,125 @@
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="3" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>45</v>
+        <v>94</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>8</v>
       </c>
       <c r="E33" s="3" t="n">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="D34" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E34" s="3" t="n">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E35" s="3" t="n">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E36" s="3" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E37" s="3" t="n">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="B38" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E38" s="3" t="n">
-        <v>90</v>
-      </c>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="4"/>
+      <c r="B34" s="0"/>
+      <c r="C34" s="0"/>
+      <c r="D34" s="0"/>
+      <c r="E34" s="0"/>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="4"/>
+      <c r="B35" s="0"/>
+      <c r="C35" s="0"/>
+      <c r="D35" s="0"/>
+      <c r="E35" s="0"/>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="4"/>
+      <c r="B36" s="0"/>
+      <c r="C36" s="0"/>
+      <c r="D36" s="0"/>
+      <c r="E36" s="0"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="4"/>
+      <c r="B37" s="0"/>
+      <c r="C37" s="0"/>
+      <c r="D37" s="0"/>
+      <c r="E37" s="0"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="4"/>
+      <c r="B38" s="0"/>
+      <c r="C38" s="0"/>
+      <c r="D38" s="0"/>
+      <c r="E38" s="0"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E39" s="3" t="n">
-        <v>330</v>
-      </c>
+      <c r="A39" s="5"/>
+      <c r="B39" s="5"/>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="B40" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="C40" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E40" s="3" t="n">
-        <v>0</v>
-      </c>
+      <c r="A40" s="5"/>
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E41" s="3" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="B42" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E42" s="3" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E43" s="3" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="B44" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E44" s="3" t="n">
-        <v>90</v>
-      </c>
+      <c r="A41" s="5"/>
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="4"/>
+      <c r="B42" s="0"/>
+      <c r="C42" s="0"/>
+      <c r="D42" s="0"/>
+      <c r="E42" s="0"/>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="4"/>
+      <c r="B43" s="0"/>
+      <c r="C43" s="0"/>
+      <c r="D43" s="0"/>
+      <c r="E43" s="0"/>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="4"/>
+      <c r="B44" s="0"/>
+      <c r="C44" s="0"/>
+      <c r="D44" s="0"/>
+      <c r="E44" s="0"/>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D45" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E45" s="3" t="n">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E46" s="3" t="n">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="B47" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="C47" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E47" s="3" t="n">
-        <v>0</v>
-      </c>
+      <c r="A45" s="5"/>
+      <c r="B45" s="5"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5"/>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="4"/>
+      <c r="B46" s="0"/>
+      <c r="C46" s="0"/>
+      <c r="D46" s="0"/>
+      <c r="E46" s="0"/>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="4"/>
+      <c r="B47" s="0"/>
+      <c r="C47" s="0"/>
+      <c r="D47" s="0"/>
+      <c r="E47" s="0"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="5"/>
-      <c r="B48" s="5"/>
-      <c r="C48" s="5"/>
-      <c r="D48" s="5"/>
-      <c r="E48" s="5"/>
+      <c r="A48" s="6"/>
+      <c r="B48" s="6"/>
+      <c r="C48" s="6"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="6"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>